<commit_message>
"giant table" with fairness metric overview
</commit_message>
<xml_diff>
--- a/references/Fairness-measures-overview.xlsx
+++ b/references/Fairness-measures-overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caroline\Documents\DTU\Master_thesis\Fairness-oriented-interpretability-of-predictive-algorithms\references\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caroline\Documents\Master-Thesis\Fairness-oriented-interpretability-of-predictive-algorithms\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6554FE-E471-422C-AFE2-17B912956ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED9B603-3C9C-43B3-9B2C-B3530DF1027C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C5FA296D-0F8B-4047-B11B-3223361D1B7B}"/>
+    <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{C5FA296D-0F8B-4047-B11B-3223361D1B7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,12 +147,6 @@
     <t>Equalized Odds</t>
   </si>
   <si>
-    <t>* Seperation
-* Positive rate parity
-* Conditional procedure accuracy equality
-*Disparate mistreatment</t>
-  </si>
-  <si>
     <t>* Equal Opportunity</t>
   </si>
   <si>
@@ -338,6 +332,12 @@
   <si>
     <t xml:space="preserve">Equal PPV, NPV, FDR and FOR in both groups. 
 I.e. the probability of subjects with positive preditive value to truly belong to the positive class and the probability of subject with negative predictive value to truly belong to the negative class are equal across groups. </t>
+  </si>
+  <si>
+    <t>* Separation
+* Positive rate parity
+* Conditional procedure accuracy equality
+*Disparate mistreatment</t>
   </si>
 </sst>
 </file>
@@ -757,28 +757,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D9494E-D880-449E-978D-3F7FB5F6B341}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="88" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.44140625" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" customWidth="1"/>
+    <col min="4" max="4" width="33.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.453125" customWidth="1"/>
+    <col min="6" max="6" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -800,7 +800,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>11</v>
@@ -809,7 +809,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>13</v>
@@ -820,7 +820,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -846,18 +846,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>15</v>
@@ -869,7 +869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -880,10 +880,10 @@
         <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
         <v>21</v>
@@ -892,7 +892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -902,21 +902,21 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>54</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>23</v>
@@ -925,15 +925,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>27</v>
@@ -948,7 +948,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="6"/>
@@ -958,21 +958,21 @@
       <c r="G10" s="8"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>23</v>
@@ -981,21 +981,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="G12" t="s">
         <v>23</v>
@@ -1004,21 +1004,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" t="s">
         <v>23</v>
@@ -1027,7 +1027,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="6"/>
@@ -1037,18 +1037,18 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="D15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="G15" t="s">
         <v>23</v>
@@ -1057,15 +1057,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="G16" t="s">
         <v>23</v>

</xml_diff>